<commit_message>
Item price added / Item no more record its owner
</commit_message>
<xml_diff>
--- a/StreamingAssets/Items.xlsx
+++ b/StreamingAssets/Items.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
   <si>
     <t>唯一标识符</t>
   </si>
@@ -30,10 +30,20 @@
     <t>属性加成比例，需填写小数</t>
   </si>
   <si>
+    <t>购买价格</t>
+  </si>
+  <si>
     <t>效果持续回合数，瞬发效果填0</t>
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>第一、二行</t>
     </r>
     <r>
@@ -97,6 +107,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>第三行此列之前</t>
     </r>
     <r>
@@ -138,6 +155,9 @@
   </si>
   <si>
     <t>KindnessScale</t>
+  </si>
+  <si>
+    <t>Price</t>
   </si>
   <si>
     <t>LastRound</t>
@@ -1161,23 +1181,23 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.56637168141593" defaultRowHeight="13.5" outlineLevelRow="5"/>
   <cols>
     <col min="1" max="1" width="11.3097345132743" style="1" customWidth="1"/>
     <col min="2" max="6" width="8.56637168141593" style="1" customWidth="1"/>
-    <col min="7" max="10" width="14.5398230088496" style="1" customWidth="1"/>
-    <col min="11" max="11" width="29.6637168141593" style="1" customWidth="1"/>
-    <col min="12" max="12" width="51.1769911504425" style="2" customWidth="1"/>
-    <col min="13" max="16384" width="8.56637168141593" style="1" customWidth="1"/>
+    <col min="7" max="11" width="14.5398230088496" style="1" customWidth="1"/>
+    <col min="12" max="12" width="29.6637168141593" style="1" customWidth="1"/>
+    <col min="13" max="13" width="51.1769911504425" style="2" customWidth="1"/>
+    <col min="14" max="16384" width="8.56637168141593" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:13">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1193,74 +1213,83 @@
       <c r="K1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="M1" s="4" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:13">
       <c r="A2" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>6</v>
-      </c>
       <c r="G2" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:13">
       <c r="A3" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L3" s="2" t="s">
         <v>21</v>
       </c>
+      <c r="L3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:13">
       <c r="A4" s="1">
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C4" s="1">
         <v>1</v>
@@ -1287,18 +1316,21 @@
         <v>0.1</v>
       </c>
       <c r="K4" s="1">
+        <v>20</v>
+      </c>
+      <c r="L4" s="1">
         <v>6</v>
       </c>
-      <c r="L4" s="2" t="s">
-        <v>23</v>
+      <c r="M4" s="2" t="s">
+        <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:13">
       <c r="A5" s="1">
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C5" s="1">
         <v>0</v>
@@ -1325,18 +1357,21 @@
         <v>0</v>
       </c>
       <c r="K5" s="1">
+        <v>30</v>
+      </c>
+      <c r="L5" s="1">
         <v>5</v>
       </c>
-      <c r="L5" s="2" t="s">
-        <v>25</v>
+      <c r="M5" s="2" t="s">
+        <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:13">
       <c r="A6" s="1">
         <v>3</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C6" s="1">
         <v>0</v>
@@ -1363,10 +1398,13 @@
         <v>0.05</v>
       </c>
       <c r="K6" s="1">
+        <v>50</v>
+      </c>
+      <c r="L6" s="1">
         <v>4</v>
       </c>
-      <c r="L6" s="2" t="s">
-        <v>27</v>
+      <c r="M6" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>